<commit_message>
DP: create_forecast_basic - fututre - taz_demo_pls_2020_and_pre_growth_till_2050.xlsx - use from Intermediates
</commit_message>
<xml_diff>
--- a/create_forecast_basic/future/JTMT/Intermediates/240501_pop_2025_jtmt.xlsx
+++ b/create_forecast_basic/future/JTMT/Intermediates/240501_pop_2025_jtmt.xlsx
@@ -9489,7 +9489,7 @@
       </c>
       <c r="C218" t="inlineStr"/>
       <c r="D218" t="n">
-        <v>23035.21100990956</v>
+        <v>23381.28486186079</v>
       </c>
       <c r="E218" t="inlineStr"/>
       <c r="F218" t="inlineStr"/>
@@ -9517,7 +9517,7 @@
       </c>
       <c r="C219" t="inlineStr"/>
       <c r="D219" t="n">
-        <v>9763.8748138847</v>
+        <v>9260.656767832284</v>
       </c>
       <c r="E219" t="inlineStr"/>
       <c r="F219" t="inlineStr"/>
@@ -9545,7 +9545,7 @@
       </c>
       <c r="C220" t="inlineStr"/>
       <c r="D220" t="n">
-        <v>10459.76068314218</v>
+        <v>10616.90487724337</v>
       </c>
       <c r="E220" t="inlineStr"/>
       <c r="F220" t="inlineStr"/>

</xml_diff>